<commit_message>
add code for different DOM structure that they use to guard malicious web scraping
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -537,7 +537,7 @@
           <t>missing</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="J2" s="3" t="inlineStr">
         <is>
           <t>missing</t>
         </is>
@@ -551,11 +551,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>this paper focuses on climate anxiety and its role in the psychology of climate change, compared with responses to the covid-19 global pandemic. four psychological hypotheses for why we do not act on climate change will be reviewed, and the role of anxiety for each, as well as potential solutions. different types of climate anxiety both inside and outside the clinic will be explored, along with associated defence mechanisms and treatment.keywords: climate anxiety, climate change, psychoanalysis, post-traumatic stress disorder, ecological trauma</t>
+          <t>this paper focuses on climate anxiety and its role in the psychology of climate change, compared with responses to the covid-19 global pandemic. four psychological hypotheses for why we do not act on climate change will be reviewed, and the role of anxiety for each, as well as potential solutions. different types of climate anxiety both inside and outside the clinic will be explored, along with associated defence mechanisms and treatment.
+keywords: climate anxiety, climate change, psychoanalysis, post-traumatic stress disorder, ecological trauma</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
@@ -587,7 +588,7 @@
           <t>missing</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="J3" s="3" t="inlineStr">
         <is>
           <t>missing</t>
         </is>
@@ -601,11 +602,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>we assess evidence relevant to earth's equilibrium climate sensitivity per doubling of atmospheric co2, characterized by an effective sensitivity s. this evidence includes feedback process understanding, the historical climate record, and the paleoclimate record. an s value lower than 2 k is difficult to reconcile with any of the three lines of evidence. the amount of cooling during the last glacial maximum provides strong evidence against values of s greater than 4.5 k. other lines of evidence in combination also show that this is relatively unlikely. we use a bayesian approach to produce a probability density function (pdf) for s given all the evidence, including tests of robustness to difficult‐to‐quantify uncertainties and different priors. the 66% range is 2.6–3.9 k for our baseline calculation and remains within 2.3–4.5 k under the robustness tests; corresponding 5–95% ranges are 2.3–4.7 k, bounded by 2.0–5.7 k (although such high‐confidence ranges should be regarded more cautiously). this indicates a stronger constraint on s than reported in past assessments, by lifting the low end of the range. this narrowing occurs because the three lines of evidence agree and are judged to be largely independent and because of greater confidence in understanding feedback processes and in combining evidence. we identify promising avenues for further narrowing the range in s, in particular using comprehensive models and process understanding to address limitations in the traditional forcing‐feedback paradigm for interpreting past changes.keywords: climate, climate sensitivity, global warming, bayesian methods</t>
+          <t>we assess evidence relevant to earth's equilibrium climate sensitivity per doubling of atmospheric co2, characterized by an effective sensitivity s. this evidence includes feedback process understanding, the historical climate record, and the paleoclimate record. an s value lower than 2 k is difficult to reconcile with any of the three lines of evidence. the amount of cooling during the last glacial maximum provides strong evidence against values of s greater than 4.5 k. other lines of evidence in combination also show that this is relatively unlikely. we use a bayesian approach to produce a probability density function (pdf) for s given all the evidence, including tests of robustness to difficult‐to‐quantify uncertainties and different priors. the 66% range is 2.6–3.9 k for our baseline calculation and remains within 2.3–4.5 k under the robustness tests; corresponding 5–95% ranges are 2.3–4.7 k, bounded by 2.0–5.7 k (although such high‐confidence ranges should be regarded more cautiously). this indicates a stronger constraint on s than reported in past assessments, by lifting the low end of the range. this narrowing occurs because the three lines of evidence agree and are judged to be largely independent and because of greater confidence in understanding feedback processes and in combining evidence. we identify promising avenues for further narrowing the range in s, in particular using comprehensive models and process understanding to address limitations in the traditional forcing‐feedback paradigm for interpreting past changes.
+keywords: climate, climate sensitivity, global warming, bayesian methods</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1627</v>
+        <v>1628</v>
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
@@ -637,7 +639,7 @@
           <t>present</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="J4" s="3" t="inlineStr">
         <is>
           <t>missing</t>
         </is>
@@ -651,11 +653,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>this article provides a stocktake of the adaptation literature between 2013 and 2019 to better understand how adaptation responses affect risk under the particularly challenging conditions of compound climate events. across 39 countries, 45 response types to compound hazards display anticipatory (9%), reactive (33%), and maladaptive (41%) characteristics, as well as hard (18%) and soft (68%) limits to adaptation. low income, food insecurity, and access to institutional resources and finance are the most prominent of 23 vulnerabilities observed to negatively affect responses. risk for food security, health, livelihoods, and economic outputs are commonly associated risks driving responses. narrow geographical and sectoral foci of the literature highlight important conceptual, sectoral, and geographic areas for future research to better understand the way responses shape risk. when responses are integrated within climate risk assessment and management, there is greater potential to advance the urgency of response and safeguards for the most vulnerable.subject areas: earth sciences, climatology, safety engineering, business, decision science</t>
+          <t>this article provides a stocktake of the adaptation literature between 2013 and 2019 to better understand how adaptation responses affect risk under the particularly challenging conditions of compound climate events. across 39 countries, 45 response types to compound hazards display anticipatory (9%), reactive (33%), and maladaptive (41%) characteristics, as well as hard (18%) and soft (68%) limits to adaptation. low income, food insecurity, and access to institutional resources and finance are the most prominent of 23 vulnerabilities observed to negatively affect responses. risk for food security, health, livelihoods, and economic outputs are commonly associated risks driving responses. narrow geographical and sectoral foci of the literature highlight important conceptual, sectoral, and geographic areas for future research to better understand the way responses shape risk. when responses are integrated within climate risk assessment and management, there is greater potential to advance the urgency of response and safeguards for the most vulnerable.
+subject areas: earth sciences, climatology, safety engineering, business, decision science</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1155</v>
+        <v>1156</v>
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
@@ -687,7 +690,7 @@
           <t>missing</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
+      <c r="J5" s="3" t="inlineStr">
         <is>
           <t>missing</t>
         </is>
@@ -701,11 +704,16 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>background:climate change has been shown to be directly linked to multiple physiological sequelae and to impact health consequences. however, the impact of climate change on mental health globally, particularly among vulnerable populations, is less well understood.objective:to explore the mental health impacts of climate change in vulnerable populations globally.methods:we performed an integrative literature review to identify published articles that addressed the research question: what are the mental health impacts of climate change among vulnerable populations globally? the vulnerable populations conceptual model served as a theoretical model during the review process and data synthesis.findings/results:one hundred and four articles were selected for inclusion in this review after a comprehensive review of 1828 manuscripts. articles were diverse in scope and populations addressed. land-vulnerable persons (either due to occupation or geographic location), indigenous persons, children, older adults, and climate migrants were among the vulnerable populations whose mental health was most impacted by climate change. the most prevalent mental health responses to climate change included solastalgia, suicidality, depression, anxiety/eco-anxiety, ptsd, substance use, insomnia, and behavioral disturbance.conclusions:mental health professionals including physicians, nurses, physician assistants and other healthcare providers have the opportunity to mitigate the mental health impacts of climate change among vulnerable populations through assessment, preventative education and care. an inclusive and trauma-informed response to climate-related disasters, use of validated measures of mental health, and a long-term therapeutic relationship that extends beyond the immediate consequences of climate change-related events are approaches to successful mental health care in a climate-changing world.keywords: mental health, climate change and health, anxiety, post-traumatic stress disorder, solastalgia, ecoanxiety</t>
+          <t>background:
+climate change has been shown to be directly linked to multiple physiological sequelae and to impact health consequences. however, the impact of climate change on mental health globally, particularly among vulnerable populations, is less well understood.objective:
+to explore the mental health impacts of climate change in vulnerable populations globally.methods:
+we performed an integrative literature review to identify published articles that addressed the research question: what are the mental health impacts of climate change among vulnerable populations globally? the vulnerable populations conceptual model served as a theoretical model during the review process and data synthesis.findings/results:
+one hundred and four articles were selected for inclusion in this review after a comprehensive review of 1828 manuscripts. articles were diverse in scope and populations addressed. land-vulnerable persons (either due to occupation or geographic location), indigenous persons, children, older adults, and climate migrants were among the vulnerable populations whose mental health was most impacted by climate change. the most prevalent mental health responses to climate change included solastalgia, suicidality, depression, anxiety/eco-anxiety, ptsd, substance use, insomnia, and behavioral disturbance.conclusions:
+mental health professionals including physicians, nurses, physician assistants and other healthcare providers have the opportunity to mitigate the mental health impacts of climate change among vulnerable populations through assessment, preventative education and care. an inclusive and trauma-informed response to climate-related disasters, use of validated measures of mental health, and a long-term therapeutic relationship that extends beyond the immediate consequences of climate change-related events are approaches to successful mental health care in a climate-changing world.keywords: mental health, climate change and health, anxiety, post-traumatic stress disorder, solastalgia, ecoanxiety</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>2029</v>
+        <v>2034</v>
       </c>
       <c r="D6" s="2" t="inlineStr">
         <is>
@@ -737,9 +745,677 @@
           <t>missing</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>missing</t>
+      <c r="J6" s="3" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC10977893/</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>urban agglomerations are emerging as new regional units for national participation in global competition and the international division of labor. however, they face increasingly severe resource and eco-environment pressures during urbanization. the coordination of the relationship between urbanization and the eco-environment has attracted global attention. in this study, we used coupling coordination degree and vector autoregression models to examine the dynamic evolution, coupling relationships, coordinated development patterns, and interaction mechanisms between urbanization and the eco-environment. the results indicate that: (1) the level of urbanization in the chengdu-chongqing urban agglomeration was relatively low, and the region showed a good eco-environment background. however, rapid urbanization is gradually straining the carrying capacity of the eco-environment. (2) a close and stable coupling relationship exists between urbanization and the eco-environment, which has reached an advanced coupling stage. the status of coordinated development among cities differs considerably, and multiple stable forms may exist simultaneously. (3) urbanization has a substantial impact on environmental changes, whereas the restrictive effect of the eco-environment on urbanization development is not particularly notable. (4) various interactive relationships exist between the urbanization and eco-environment subsystems, including positive promotion and negative constraint effects. the positive promotion effect mainly manifests between the economic, social, and ecological response subsystems, while the negative constraint effect is most evident in the mutual coercion and inhibition between the regional urbanization, economic urbanization, ecological status, and ecological pressure subsystems. these findings have important policy implications for decision makers exploring the path of coordinated and sustainable development in urbanization and the eco-environment in urban agglomerations.</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>2009</v>
+      </c>
+      <c r="D7" s="2" t="inlineStr">
+        <is>
+          <t>Length: OK</t>
+        </is>
+      </c>
+      <c r="E7" s="3" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+      <c r="F7" s="2" t="inlineStr">
+        <is>
+          <t>present</t>
+        </is>
+      </c>
+      <c r="G7" s="3" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+      <c r="H7" s="3" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+      <c r="I7" s="3" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+      <c r="J7" s="3" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC8446952/</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>the coronavirus disease 2019 (covid‐19) pandemic has drastically changed work styles and environments. given the coexistence of work in the office and work from home (wfh) in the future, studies are needed to identify ways to increase productivity when working in both places. we conducted a questionnaire survey and environment measurements of 916 workers in 22 offices across 2 weeks in november–december 2020 in japan. while average workdays at the offices decreased from 4.9 to 3.9 days/week, those at homes increased from 0.1 to 1.1 days/week due to covid‐19, indicating an increase in the relative importance of wfh. compared to the office, the satisfaction rate was lower for lighting, spatial, and information technology (it) environments, but higher for thermal, air, and sound environments at home. although it was easier to concentrate on work and to refresh at home, workers experienced challenges associated with business communication from home. meanwhile, in the office, satisfaction with covid‐19 countermeasures was significantly associated with work productivity. furthermore, lower pm2.5 concentration was associated with greater satisfaction with covid‐19 countermeasures, indicating that reducing pm2.5 may increase satisfaction with covid‐19 countermeasures and work productivity. we expect these findings will help improve work productivity in the new normal era.
+keywords: covid‐19, pm2.5
+, productivity, work environment, work from home, work in the office</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>1481</v>
+      </c>
+      <c r="D8" s="2" t="inlineStr">
+        <is>
+          <t>Length: OK</t>
+        </is>
+      </c>
+      <c r="E8" s="3" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+      <c r="F8" s="2" t="inlineStr">
+        <is>
+          <t>present</t>
+        </is>
+      </c>
+      <c r="G8" s="3" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+      <c r="H8" s="3" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+      <c r="I8" s="3" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+      <c r="J8" s="3" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC9971900/</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>this article provides a stocktake of the adaptation literature between 2013 and 2019 to better understand how adaptation responses affect risk under the particularly challenging conditions of compound climate events. across 39 countries, 45 response types to compound hazards display anticipatory (9%), reactive (33%), and maladaptive (41%) characteristics, as well as hard (18%) and soft (68%) limits to adaptation. low income, food insecurity, and access to institutional resources and finance are the most prominent of 23 vulnerabilities observed to negatively affect responses. risk for food security, health, livelihoods, and economic outputs are commonly associated risks driving responses. narrow geographical and sectoral foci of the literature highlight important conceptual, sectoral, and geographic areas for future research to better understand the way responses shape risk. when responses are integrated within climate risk assessment and management, there is greater potential to advance the urgency of response and safeguards for the most vulnerable.
+subject areas: earth sciences, climatology, safety engineering, business, decision science</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>1156</v>
+      </c>
+      <c r="D9" s="2" t="inlineStr">
+        <is>
+          <t>Length: OK</t>
+        </is>
+      </c>
+      <c r="E9" s="2" t="inlineStr">
+        <is>
+          <t>present</t>
+        </is>
+      </c>
+      <c r="F9" s="3" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+      <c r="G9" s="3" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+      <c r="H9" s="3" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+      <c r="I9" s="3" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+      <c r="J9" s="3" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC11336597/</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>the future of food production in nigeria where smallholding agriculture is prevalent is threatened by climate change. despite the threats, nigeria has no specific plan or policy to combat it. therefore, understanding how smallholder farmers adjust to the changing climate and the factors that influence their adaptation choices will facilitate developing a policy to tackle climate change. this study therefore evaluates climate change adaptation techniques among smallholder rice farmers in kebbi state, nigeria. the study employs a simple random sampling technique to select 345 respondents. the data was analysed using multivariate probit and ordered probit regression.
+the findings revealed that marital status, literacy, farm size, farming experience, major occupation, extension visits, amount of credit, and access to climate information influenced adaptation strategy choice. furthermore, marital status, literacy, household size, farm size, extension visits, and access to climate information are crucial drivers of adoption intensity. this study concludes that smallholder rice farmers in the study area adopt several practices to cope with climate change, however, farmers’ intensity of adoption is low. this study recommends that stakeholders in the food systems in the study area should consider literacy, farm size, extension service, credits, and climate information in designing viable policies toward combating the vagaries of climate.
+keywords: climate change, adaptations, intensity, smallholder, rice farmer, nigeria</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>1536</v>
+      </c>
+      <c r="D10" s="2" t="inlineStr">
+        <is>
+          <t>Length: OK</t>
+        </is>
+      </c>
+      <c r="E10" s="2" t="inlineStr">
+        <is>
+          <t>present</t>
+        </is>
+      </c>
+      <c r="F10" s="3" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+      <c r="G10" s="3" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+      <c r="H10" s="3" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+      <c r="I10" s="3" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+      <c r="J10" s="3" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC10558031/</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>background:
+climate change has been shown to be directly linked to multiple physiological sequelae and to impact health consequences. however, the impact of climate change on mental health globally, particularly among vulnerable populations, is less well understood.objective:
+to explore the mental health impacts of climate change in vulnerable populations globally.methods:
+we performed an integrative literature review to identify published articles that addressed the research question: what are the mental health impacts of climate change among vulnerable populations globally? the vulnerable populations conceptual model served as a theoretical model during the review process and data synthesis.findings/results:
+one hundred and four articles were selected for inclusion in this review after a comprehensive review of 1828 manuscripts. articles were diverse in scope and populations addressed. land-vulnerable persons (either due to occupation or geographic location), indigenous persons, children, older adults, and climate migrants were among the vulnerable populations whose mental health was most impacted by climate change. the most prevalent mental health responses to climate change included solastalgia, suicidality, depression, anxiety/eco-anxiety, ptsd, substance use, insomnia, and behavioral disturbance.conclusions:
+mental health professionals including physicians, nurses, physician assistants and other healthcare providers have the opportunity to mitigate the mental health impacts of climate change among vulnerable populations through assessment, preventative education and care. an inclusive and trauma-informed response to climate-related disasters, use of validated measures of mental health, and a long-term therapeutic relationship that extends beyond the immediate consequences of climate change-related events are approaches to successful mental health care in a climate-changing world.keywords: mental health, climate change and health, anxiety, post-traumatic stress disorder, solastalgia, ecoanxiety</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>2034</v>
+      </c>
+      <c r="D11" s="2" t="inlineStr">
+        <is>
+          <t>Length: OK</t>
+        </is>
+      </c>
+      <c r="E11" s="2" t="inlineStr">
+        <is>
+          <t>present</t>
+        </is>
+      </c>
+      <c r="F11" s="3" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+      <c r="G11" s="3" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+      <c r="H11" s="2" t="inlineStr">
+        <is>
+          <t>present</t>
+        </is>
+      </c>
+      <c r="I11" s="3" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+      <c r="J11" s="3" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC6655584/</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>major ecological realignments are already occurring in response to climate change. to be successful, conservation strategies now need to account for geographical patterns in traits sensitive to climate change, as well as climate threats to species-level diversity. as part of an effort to provide such information, we conducted a climate vulnerability assessment that included all anadromous pacific salmon and steelhead (oncorhynchus spp.) population units listed under the u.s. endangered species act. using an expert-based scoring system, we ranked 20 attributes for the 28 listed units and 5 additional units. attributes captured biological sensitivity, or the strength of linkages between each listing unit and the present climate; climate exposure, or the magnitude of projected change in local environmental conditions; and adaptive capacity, or the ability to modify phenotypes to cope with new climatic conditions. each listing unit was then assigned one of four vulnerability categories. units ranked most vulnerable overall were chinook (o. tshawytscha) in the california central valley, coho (o. kisutch) in california and southern oregon, sockeye (o. nerka) in the snake river basin, and spring-run chinook in the interior columbia and willamette river basins. we identified units with similar vulnerability profiles using a hierarchical cluster analysis. life history characteristics, especially freshwater and estuary residence times, interplayed with gradations in exposure from south to north and from coastal to interior regions to generate landscape-level patterns within each species. nearly all listing units faced high exposures to projected increases in stream temperature, sea surface temperature, and ocean acidification, but other aspects of exposure peaked in particular regions. anthropogenic factors, especially migration barriers, habitat degradation, and hatchery influence, have reduced the adaptive capacity of most steelhead and salmon populations. enhancing adaptive capacity is essential to mitigate for the increasing threat of climate change. collectively, these results provide a framework to support recovery planning that considers climate impacts on the majority of west coast anadromous salmonids.</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>2240</v>
+      </c>
+      <c r="D12" s="2" t="inlineStr">
+        <is>
+          <t>Length: OK</t>
+        </is>
+      </c>
+      <c r="E12" s="2" t="inlineStr">
+        <is>
+          <t>present</t>
+        </is>
+      </c>
+      <c r="F12" s="2" t="inlineStr">
+        <is>
+          <t>present</t>
+        </is>
+      </c>
+      <c r="G12" s="3" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+      <c r="H12" s="3" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+      <c r="I12" s="2" t="inlineStr">
+        <is>
+          <t>present</t>
+        </is>
+      </c>
+      <c r="J12" s="3" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC10118127/</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>the climate crisis not only has significant impacts on biodiversity and the physical health of humans, but its ramifications are also affecting people’s mental health. eco-anxiety, or the emotions that emerge with the awareness of climate change and the apprehension of its detrimental effects, has been investigated in adults and adolescents, but much less attention has been given to the impacts on children’s mental health and well-being. initial evidence confirms that youth are significantly concerned about climate change, but few studies have investigated the resulting emotional responses of children and the role of their parents in tempering these, especially using qualitative methodologies. the present study used a descriptive qualitative design with a convenience sample of parents and child dyads, assessed separately. children’s (n = 15, ages 8–12 years) experiences were explored using semi-structured interviews and their parents’ (n = 12) perceptions were captured using a survey with closed and open-ended questions. a reflexive thematic analysis was used to analyze the interview data, and content analysis was used to investigate parent-child experiences. three themes emerged from the thematic analysis: 1. children’s understanding of climate change, 2. their emotional reaction to climate change, and 3. their coping mechanisms to deal with these emotions. the comparative content analysis revealed that parents who were aware that their children had concerns about climate change, had children who used more adaptive coping mechanisms. the results of this qualitative study contribute to a better understanding of children’s emotional experience of the awareness of climate change in canada and how they cope with these emotions. furthermore, the results provide insight into the role parents might play in helping their children cope with their feelings.</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>1880</v>
+      </c>
+      <c r="D13" s="2" t="inlineStr">
+        <is>
+          <t>Length: OK</t>
+        </is>
+      </c>
+      <c r="E13" s="2" t="inlineStr">
+        <is>
+          <t>present</t>
+        </is>
+      </c>
+      <c r="F13" s="3" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+      <c r="G13" s="3" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+      <c r="H13" s="2" t="inlineStr">
+        <is>
+          <t>present</t>
+        </is>
+      </c>
+      <c r="I13" s="3" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+      <c r="J13" s="3" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC11133169/</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>the term ‘environment’ is not uniformly defined in the public health sciences, which causes crucial inconsistencies in research, health policy, and practice. as we shall indicate, this is somewhat entangled with diverging pathogenic and salutogenic perspectives (research and policy priorities) concerning environmental health. we emphasise two distinct concepts of environment in use by the world health organisation. one significant way these concepts differ concerns whether the social environment is included. divergence on this matter has profound consequences for the understanding of health and disease, for measures derived from that understanding targeting health promotion and disease prevention, and consequently, for epistemic structures and concept development in scientific practice. we hope to improve the given situation in public health by uncovering these differences and by developing a fruitful way of thinking about environment. firstly, we side with the salutogenic conception of environment as a health resource (as well as a source of health risks). secondly, we subdivide the concept of environment into four health-oriented environmental categories (viz., natural, built-material, socio-cultural, and psychosocial) and we link these with other theoretical notions proposed in the health sciences literature. thirdly, we propose that in public health ‘environment’ should be understood as consisting of all extrinsic factors that influence or are influenced by the health, well-being, and development of an individual. consequently, none of the four categories should be excluded from the concept of environment. we point out the practical relevance and fruitfulness of the conception of environment as a health source and frame this in causal terms, representing individual health environments as causal networks. throughout, we side with the view that for the design of human health-promoting settings, increased attention and consideration of environmental resources of salutogenic potential is particularly pressing.
+keywords: definition of environment, environmental health determinants, human ecology, individualisation, public health, salutogenesis, social environment</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>2200</v>
+      </c>
+      <c r="D14" s="2" t="inlineStr">
+        <is>
+          <t>Length: OK</t>
+        </is>
+      </c>
+      <c r="E14" s="3" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+      <c r="F14" s="2" t="inlineStr">
+        <is>
+          <t>present</t>
+        </is>
+      </c>
+      <c r="G14" s="3" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+      <c r="H14" s="3" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+      <c r="I14" s="3" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+      <c r="J14" s="3" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC10815757/</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>the occurrence of severe and extreme weather events that have been attributed to a changed climate system and the widespread dissemination of the impacts of these events in the media can lead people to experience concern, worry, and anxiety, which we examined in two studies. in study 1, we observed that people more frequently expressed worry than anxiety about the impacts of climate change in six areas. people were more frequently worried and anxious about the effects of climate change on future generations and about societal responses (or lack of a response) to climate change. the levels of anxiety that people expressed were significantly higher than the worry people reported when anxiety was their modal response. in study 2, we observed that both climate change worry and anxiety were negatively correlated with psychological distance from climate change. overall, climate change worry and psychological distance significantly predicted climate-sustainable behaviors. our study was among the first to use developed measures of climate change worry, anxiety, and psychological distance to examine peoples’ responses across some of the possible impact and consequence areas of climate change.
+keywords: climate change, anxiety, worry, climate change impacts, consequences of climate change, psychological distance, sustainable behaviors</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>1346</v>
+      </c>
+      <c r="D15" s="2" t="inlineStr">
+        <is>
+          <t>Length: OK</t>
+        </is>
+      </c>
+      <c r="E15" s="2" t="inlineStr">
+        <is>
+          <t>present</t>
+        </is>
+      </c>
+      <c r="F15" s="3" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+      <c r="G15" s="3" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+      <c r="H15" s="2" t="inlineStr">
+        <is>
+          <t>present</t>
+        </is>
+      </c>
+      <c r="I15" s="3" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+      <c r="J15" s="3" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC9761729/</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>climate change has the greatest negative impact on low-income countries, which burdens agricultural systems. climate change and extreme weather events have caused ethiopia’s agricultural production to decline and exacerbated food insecurity over the last few decades. this study investigates whether farmers’ awareness and perceptions of climate change play a role in climate change adaptation using climate-smart agricultural practices. to collect data, 385 households in southern ethiopia were sampled using a multistage sampling. a heckman probit two-stage selection model was applied to investigate the factors influencing farmers’ perceptions to climate change and adaptation measures through adoption of climate-smart agriculture practices, complemented with key informant interviews and focused group discussions. the results indicated that most farmers (81.80%) perceived that the local climate is changing, with 71.9% reporting increased temperature and 53.15% reporting decreasing rainfall distribution. therefore, farmers attempted to apply some adaptation practices, including soil and water conservation with biological measures, improved crop varieties, agroforestry, improved breeds, cut and carry system, controlled grazing, and residue incorporation. the empirical results revealed that farmers adaptation to climate change through adoptions of csa practices was significantly influenced by education, family size, gender, landholding size, farming experience, access to climate information, training received, social membership, livestock ownership, farm income and extension services. the study found that farmers’ perceptions of climate change and variability were significantly influenced by their age, level of education, farming experience, and access to climate information, hence, the need to focus on enhancing the accuracy of weather information, strengthening extension services, and considering a gender-sensitive adaptation approach toward improving farmers’ knowledge and aspirations. agricultural policies should support the efforts of farmers to increase the reliance on climate risk and alleviate farmers’ difficulties in adopting climate-smart agriculture practices.
+keywords: climate change and variability, perceptions, climate-smart agriculture, adaptation, policy, ethiopia</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>2312</v>
+      </c>
+      <c r="D16" s="2" t="inlineStr">
+        <is>
+          <t>Length: OK</t>
+        </is>
+      </c>
+      <c r="E16" s="2" t="inlineStr">
+        <is>
+          <t>present</t>
+        </is>
+      </c>
+      <c r="F16" s="3" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+      <c r="G16" s="3" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+      <c r="H16" s="3" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+      <c r="I16" s="3" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+      <c r="J16" s="3" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC6156563/</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>changing climate will impact species’ ranges only when environmental variability directly impacts the demography of local populations. however, measurement of demographic responses to climate change has largely been limited to single species and locations. here we show that amphibian communities are responsive to climatic variability, using &gt;500,000 time-series observations for 81 species across 86 north american study areas. the effect of climate on local colonization and persistence probabilities varies among eco-regions and depends on local climate, species life-histories, and taxonomic classification. we found that local species richness is most sensitive to changes in water availability during breeding and changes in winter conditions. based on the relationships we measure, recent changes in climate cannot explain why local species richness of north american amphibians has rapidly declined. however, changing climate does explain why some populations are declining faster than others. our results provide important insights into how amphibians respond to climate and a general framework for measuring climate impacts on species richness.</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>1155</v>
+      </c>
+      <c r="D17" s="2" t="inlineStr">
+        <is>
+          <t>Length: OK</t>
+        </is>
+      </c>
+      <c r="E17" s="2" t="inlineStr">
+        <is>
+          <t>present</t>
+        </is>
+      </c>
+      <c r="F17" s="2" t="inlineStr">
+        <is>
+          <t>present</t>
+        </is>
+      </c>
+      <c r="G17" s="3" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+      <c r="H17" s="3" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+      <c r="I17" s="3" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+      <c r="J17" s="3" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC9324041/</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>in this study, we first found that the few and sparse meteorological stations used in earlier comprehensive studies of building climate zoning in a complicated terrain area like chongqing, china, may lead to the inapplicability of building energy efficiency standards in some areas. to address this issue, the study used daily data from 1908 extremely dense surface meteorological stations from 2011 to 2020 in chongqing, china. in order to conduct fine zoning of building climate in chongqing, china, gb50176-2016 and ashrae standard 169-2021 were employed, respectively. the findings indicated that by using the ashrae standard, the entire chongqing region was classified into five climate zones. the chongqing region was categorized into three different climate zones using china gb50176-2016: cold zone (cz), hot summer and cold winter zone (hscwz), and mild zone (mz). not to be overlooked is the mz (china’s gb50176-2016)/mixed-humid zone (ashrae standard), which is primarily situated at higher elevations in the southeast and northeast of chongqing. in comparison to the hscwz/warm-humid zone, these zones have drastically different building energy efficiency regulations and approaches. according to preliminary projections, improved building climate zoning will to some extent increase building energy efficiency and reduce emissions in chongqing. finally, this study case can be replicated in different regions with complicated terrain.
+keywords: ashrae standard 169-2021, gb50176-2016, heating degree-days, cooling degree-days</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>1538</v>
+      </c>
+      <c r="D18" s="2" t="inlineStr">
+        <is>
+          <t>Length: OK</t>
+        </is>
+      </c>
+      <c r="E18" s="2" t="inlineStr">
+        <is>
+          <t>present</t>
+        </is>
+      </c>
+      <c r="F18" s="3" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+      <c r="G18" s="3" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+      <c r="H18" s="3" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+      <c r="I18" s="3" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+      <c r="J18" s="3" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC10463182/</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>introduction
+radon is a major indoor air pollutant that poses a significant risk of lung cancer to those exposed in their homes. while mitigation of high radon levels in homes has been shown to be effective, home mitigation rates remain low. this study examines the barriers and facilitators to radon mitigation in homes from the perspectives of authorities responsible for radon risk management, the mitigation industry (contractors), and residents in four european countries (belgium, ireland, slovenia, and the uk) with high radon risks and low mitigation rates.methods
+a multi-method approach was used to gather data from various stakeholders, including online surveys, content analysis of legal documents, group interviews, workshops, and focus groups.results
+authorities, contractors, and residents identified various facilitators to radon mitigation, including legal requirements for mitigation, awareness campaigns, low mitigation costs, availability of financial support, accreditation of mitigation contractors, and a perception of radon as a health threat. however, barriers to mitigation were also identified, such as a lack of awareness, fragmented mitigation processes, and inadequate communication between stakeholders.discussion
+the study highlights the complexity of the radon mitigation process and suggests that interventions aimed at increasing mitigation rates should target stakeholders beyond just residents, such as constructors, health professionals, and policy makers. an integrated approach to radon mitigation, from policy to provision, is necessary to effectively lower levels of this indoor air pollutant.keywords: radon, lung cancer, risk, mitigation, barriers, facilitators</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>1705</v>
+      </c>
+      <c r="D19" s="2" t="inlineStr">
+        <is>
+          <t>Length: OK</t>
+        </is>
+      </c>
+      <c r="E19" s="3" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+      <c r="F19" s="3" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+      <c r="G19" s="3" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+      <c r="H19" s="3" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+      <c r="I19" s="3" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+      <c r="J19" s="2" t="inlineStr">
+        <is>
+          <t>present</t>
         </is>
       </c>
     </row>

</xml_diff>